<commit_message>
[ProjRech] CS classiques : rédaction
</commit_message>
<xml_diff>
--- a/master2/output/heads_compare.xlsx
+++ b/master2/output/heads_compare.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\master2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9275BAC-C8B8-4CAB-BC31-98345A378FFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C69278-287E-4989-B7BA-753E2A31F834}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7140" yWindow="945" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="New Compare Corpus Trans" sheetId="5" r:id="rId1"/>
-    <sheet name="New Trans vs Disc" sheetId="6" r:id="rId2"/>
-    <sheet name="Best TRANS for each" sheetId="1" r:id="rId3"/>
-    <sheet name="Compare c1n, c2nA, c2nB" sheetId="2" r:id="rId4"/>
-    <sheet name="all" sheetId="4" r:id="rId5"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId6"/>
-    <sheet name="Feuil4" sheetId="7" r:id="rId7"/>
+    <sheet name="Trans" sheetId="7" r:id="rId1"/>
+    <sheet name="New Compare Corpus Trans" sheetId="5" r:id="rId2"/>
+    <sheet name="New Trans vs Disc" sheetId="6" r:id="rId3"/>
+    <sheet name="Best TRANS for each" sheetId="1" r:id="rId4"/>
+    <sheet name="Compare c1n, c2nA, c2nB" sheetId="2" r:id="rId5"/>
+    <sheet name="all" sheetId="4" r:id="rId6"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="439">
   <si>
     <t>c1n</t>
   </si>
@@ -1345,6 +1345,12 @@
   </si>
   <si>
     <t>% communs</t>
+  </si>
+  <si>
+    <t>Legallois</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -1637,7 +1643,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -1792,6 +1798,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2132,12 +2139,633 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D1D830-E714-4FAA-8A52-7865C299F082}">
+  <dimension ref="A1:B125"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="54" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="54" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+    </row>
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="54"/>
+    </row>
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="54"/>
+    </row>
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="54"/>
+    </row>
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="54"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="B28" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="54" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="54"/>
+    </row>
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="54"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="54" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+    </row>
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="54"/>
+    </row>
+    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="54"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" s="82"/>
+    </row>
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="54" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="54"/>
+    </row>
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="54"/>
+    </row>
+    <row r="66" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="54"/>
+    </row>
+    <row r="70" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="54"/>
+    </row>
+    <row r="73" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="54"/>
+    </row>
+    <row r="75" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="54" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="54"/>
+    </row>
+    <row r="80" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="54"/>
+    </row>
+    <row r="81" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="54"/>
+    </row>
+    <row r="83" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="54"/>
+    </row>
+    <row r="90" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="54"/>
+    </row>
+    <row r="98" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="54" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="54" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="54"/>
+    </row>
+    <row r="108" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="54"/>
+    </row>
+    <row r="111" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="54"/>
+    </row>
+    <row r="114" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="54"/>
+    </row>
+    <row r="116" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="54"/>
+    </row>
+    <row r="119" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="54"/>
+    </row>
+    <row r="123" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="54"/>
+    </row>
+    <row r="125" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="53">
+        <f>COUNTA(A2:A124)</f>
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3292D10D-54FC-45AA-B3B1-4B4A0A393270}">
   <dimension ref="A1:P126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N126" sqref="N126"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A1:A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6975,11 +7603,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AB4A7B-5301-4E48-9A7E-EF1BF9F68963}">
   <dimension ref="A1:F364"/>
   <sheetViews>
-    <sheetView topLeftCell="A333" workbookViewId="0">
+    <sheetView topLeftCell="A330" workbookViewId="0">
       <selection activeCell="E358" sqref="E358"/>
     </sheetView>
   </sheetViews>
@@ -10911,7 +11539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD67"/>
   <sheetViews>
@@ -14896,7 +15524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
@@ -15863,7 +16491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FBEC09-68B9-445B-A9FE-5B8FD50334A6}">
   <dimension ref="A1:F61"/>
   <sheetViews>
@@ -16448,12 +17076,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16753,21 +17381,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515E0600-FBC5-492B-B5EB-9D88583EFF82}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A372">
-    <sortCondition ref="A1"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[ProjRech] V2 envoyée, fouille KO (2e essai).
</commit_message>
<xml_diff>
--- a/master2/output/heads_compare.xlsx
+++ b/master2/output/heads_compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\master2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C69278-287E-4989-B7BA-753E2A31F834}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC08CB69-936A-49CF-80FA-B9D9840D17ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="0" windowWidth="19605" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trans" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2477" uniqueCount="441">
   <si>
     <t>c1n</t>
   </si>
@@ -1351,6 +1351,12 @@
   </si>
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>Corpus + Sig</t>
+  </si>
+  <si>
+    <t>Corpus + Leg.</t>
   </si>
 </sst>
 </file>
@@ -2142,7 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D1D830-E714-4FAA-8A52-7865C299F082}">
   <dimension ref="A1:B125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
@@ -2761,11 +2767,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3292D10D-54FC-45AA-B3B1-4B4A0A393270}">
-  <dimension ref="A1:P126"/>
+  <dimension ref="A1:X126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A1:A125"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W125" sqref="W125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,7 +2787,7 @@
     <col min="17" max="16384" width="11" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>182</v>
       </c>
@@ -2825,8 +2831,26 @@
         <v>421</v>
       </c>
       <c r="P1" s="61"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R1" s="68" t="s">
+        <v>417</v>
+      </c>
+      <c r="S1" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="T1" s="75" t="s">
+        <v>182</v>
+      </c>
+      <c r="U1" s="66" t="s">
+        <v>421</v>
+      </c>
+      <c r="V1" s="66" t="s">
+        <v>439</v>
+      </c>
+      <c r="W1" s="66" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>52</v>
       </c>
@@ -2858,8 +2882,23 @@
         <v>59</v>
       </c>
       <c r="P2" s="60"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R2" s="69">
+        <v>1</v>
+      </c>
+      <c r="S2" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="76">
+        <v>1</v>
+      </c>
+      <c r="U2" s="64">
+        <v>59</v>
+      </c>
+      <c r="V2" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>181</v>
       </c>
@@ -2894,8 +2933,19 @@
       <c r="P3" s="60" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R3" s="70">
+        <f>R2+1</f>
+        <v>2</v>
+      </c>
+      <c r="S3" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="T3" s="77">
+        <v>1</v>
+      </c>
+      <c r="U3" s="65"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
         <v>2</v>
       </c>
@@ -2940,8 +2990,27 @@
         <v>178</v>
       </c>
       <c r="P4" s="60"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R4" s="69">
+        <f t="shared" ref="R4:R67" si="1">R3+1</f>
+        <v>3</v>
+      </c>
+      <c r="S4" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="76">
+        <v>1</v>
+      </c>
+      <c r="U4" s="64">
+        <v>178</v>
+      </c>
+      <c r="V4" s="54">
+        <v>1</v>
+      </c>
+      <c r="W4" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>36</v>
       </c>
@@ -2986,8 +3055,24 @@
         <v>44</v>
       </c>
       <c r="P5" s="60"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R5" s="70">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="S5" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" s="77">
+        <v>1</v>
+      </c>
+      <c r="U5" s="65">
+        <v>44</v>
+      </c>
+      <c r="V5" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>14</v>
       </c>
@@ -3031,8 +3116,24 @@
       <c r="O6" s="64">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R6" s="69">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="S6" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="T6" s="76">
+        <v>1</v>
+      </c>
+      <c r="U6" s="64">
+        <v>16</v>
+      </c>
+      <c r="V6" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>4</v>
       </c>
@@ -3076,8 +3177,24 @@
       <c r="O7" s="65">
         <v>246</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R7" s="70">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="S7" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="77">
+        <v>1</v>
+      </c>
+      <c r="U7" s="65">
+        <v>246</v>
+      </c>
+      <c r="V7" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>56</v>
       </c>
@@ -3115,8 +3232,27 @@
       <c r="O8" s="64">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R8" s="69">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="S8" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" s="76">
+        <v>1</v>
+      </c>
+      <c r="U8" s="64">
+        <v>78</v>
+      </c>
+      <c r="V8" s="54">
+        <v>1</v>
+      </c>
+      <c r="W8" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>84</v>
       </c>
@@ -3150,8 +3286,24 @@
       <c r="O9" s="65">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R9" s="70">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="S9" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="T9" s="77">
+        <v>1</v>
+      </c>
+      <c r="U9" s="65">
+        <v>83</v>
+      </c>
+      <c r="V9" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>180</v>
       </c>
@@ -3190,8 +3342,24 @@
         <v>31</v>
       </c>
       <c r="P10" s="60"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R10" s="69">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="S10" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="T10" s="76">
+        <v>1</v>
+      </c>
+      <c r="U10" s="64">
+        <v>31</v>
+      </c>
+      <c r="V10" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
         <v>62</v>
       </c>
@@ -3226,8 +3394,24 @@
         <v>890</v>
       </c>
       <c r="P11" s="60"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R11" s="70">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="S11" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" s="77">
+        <v>1</v>
+      </c>
+      <c r="U11" s="65">
+        <v>890</v>
+      </c>
+      <c r="V11" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>179</v>
       </c>
@@ -3260,8 +3444,24 @@
         <v>209</v>
       </c>
       <c r="P12" s="60"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R12" s="69">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="S12" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="T12" s="76">
+        <v>1</v>
+      </c>
+      <c r="U12" s="64">
+        <v>209</v>
+      </c>
+      <c r="V12" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>32</v>
       </c>
@@ -3301,8 +3501,24 @@
         <v>44</v>
       </c>
       <c r="P13" s="60"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R13" s="70">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="S13" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="T13" s="77">
+        <v>1</v>
+      </c>
+      <c r="U13" s="65">
+        <v>44</v>
+      </c>
+      <c r="V13" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C14" s="57" t="s">
         <v>112</v>
       </c>
@@ -3327,8 +3543,19 @@
         <v>18</v>
       </c>
       <c r="P14" s="60"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R14" s="69">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="S14" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="T14" s="76"/>
+      <c r="U14" s="64">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
         <v>178</v>
       </c>
@@ -3363,8 +3590,27 @@
         <v>143</v>
       </c>
       <c r="P15" s="60"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R15" s="70">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="S15" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="T15" s="77">
+        <v>1</v>
+      </c>
+      <c r="U15" s="65">
+        <v>143</v>
+      </c>
+      <c r="V15" s="54">
+        <v>1</v>
+      </c>
+      <c r="W15" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D16" s="57" t="s">
         <v>177</v>
       </c>
@@ -3391,8 +3637,22 @@
         <v>248</v>
       </c>
       <c r="P16" s="60"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R16" s="69">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="S16" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="T16" s="76"/>
+      <c r="U16" s="64">
+        <v>248</v>
+      </c>
+      <c r="X16" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
         <v>44</v>
       </c>
@@ -3432,8 +3692,27 @@
         <v>132</v>
       </c>
       <c r="P17" s="60"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R17" s="70">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="S17" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="T17" s="77">
+        <v>1</v>
+      </c>
+      <c r="U17" s="65">
+        <v>132</v>
+      </c>
+      <c r="V17" s="54">
+        <v>1</v>
+      </c>
+      <c r="W17" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
         <v>13</v>
       </c>
@@ -3478,8 +3757,24 @@
         <v>2</v>
       </c>
       <c r="P18" s="60"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R18" s="69">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="S18" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="T18" s="76">
+        <v>1</v>
+      </c>
+      <c r="U18" s="64">
+        <v>2</v>
+      </c>
+      <c r="V18" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C19" s="57" t="s">
         <v>18</v>
       </c>
@@ -3514,8 +3809,19 @@
         <v>73</v>
       </c>
       <c r="P19" s="60"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R19" s="70">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="S19" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="T19" s="77"/>
+      <c r="U19" s="65">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>18</v>
       </c>
@@ -3554,8 +3860,24 @@
         <v>16</v>
       </c>
       <c r="P20" s="60"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R20" s="69">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="S20" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="T20" s="76">
+        <v>1</v>
+      </c>
+      <c r="U20" s="64">
+        <v>16</v>
+      </c>
+      <c r="V20" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21" s="57" t="s">
         <v>175</v>
       </c>
@@ -3585,8 +3907,19 @@
         <v>3</v>
       </c>
       <c r="P21" s="60"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R21" s="70">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="S21" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="T21" s="77"/>
+      <c r="U21" s="65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C22" s="57" t="s">
         <v>107</v>
       </c>
@@ -3610,8 +3943,17 @@
       <c r="P22" s="60" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R22" s="69">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="S22" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="T22" s="76"/>
+      <c r="U22" s="64"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="54" t="s">
         <v>91</v>
       </c>
@@ -3644,8 +3986,24 @@
         <v>26</v>
       </c>
       <c r="P23" s="60"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R23" s="70">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="S23" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="T23" s="77">
+        <v>1</v>
+      </c>
+      <c r="U23" s="65">
+        <v>26</v>
+      </c>
+      <c r="V23" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D24" s="57" t="s">
         <v>174</v>
       </c>
@@ -3672,8 +4030,19 @@
         <v>68</v>
       </c>
       <c r="P24" s="60"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R24" s="69">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="S24" s="72" t="s">
+        <v>174</v>
+      </c>
+      <c r="T24" s="76"/>
+      <c r="U24" s="64">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D25" s="57" t="s">
         <v>173</v>
       </c>
@@ -3705,8 +4074,19 @@
       <c r="P25" s="60" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R25" s="70">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="S25" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="T25" s="77"/>
+      <c r="U25" s="65">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
         <v>23</v>
       </c>
@@ -3751,8 +4131,24 @@
         <v>39</v>
       </c>
       <c r="P26" s="60"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R26" s="69">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="S26" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="T26" s="76">
+        <v>1</v>
+      </c>
+      <c r="U26" s="64">
+        <v>39</v>
+      </c>
+      <c r="V26" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
         <v>172</v>
       </c>
@@ -3782,8 +4178,24 @@
         <v>8</v>
       </c>
       <c r="P27" s="60"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R27" s="70">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="S27" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="T27" s="77">
+        <v>1</v>
+      </c>
+      <c r="U27" s="65">
+        <v>8</v>
+      </c>
+      <c r="V27" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
         <v>171</v>
       </c>
@@ -3814,8 +4226,27 @@
         <v>51</v>
       </c>
       <c r="P28" s="60"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R28" s="69">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="S28" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="T28" s="76">
+        <v>1</v>
+      </c>
+      <c r="U28" s="64">
+        <v>51</v>
+      </c>
+      <c r="V28" s="54">
+        <v>1</v>
+      </c>
+      <c r="W28" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
         <v>170</v>
       </c>
@@ -3855,8 +4286,24 @@
         <v>7</v>
       </c>
       <c r="P29" s="60"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R29" s="70">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="S29" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="T29" s="77">
+        <v>1</v>
+      </c>
+      <c r="U29" s="65">
+        <v>7</v>
+      </c>
+      <c r="V29" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D30" s="57" t="s">
         <v>125</v>
       </c>
@@ -3883,8 +4330,19 @@
         <v>44</v>
       </c>
       <c r="P30" s="60"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R30" s="69">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="S30" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="T30" s="76"/>
+      <c r="U30" s="64">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
         <v>31</v>
       </c>
@@ -3927,8 +4385,19 @@
       <c r="P31" s="63" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R31" s="70">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="S31" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="T31" s="77">
+        <v>1</v>
+      </c>
+      <c r="U31" s="65"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C32" s="57" t="s">
         <v>57</v>
       </c>
@@ -3952,8 +4421,17 @@
       <c r="P32" s="60" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R32" s="69">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="S32" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="T32" s="76"/>
+      <c r="U32" s="64"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
         <v>3</v>
       </c>
@@ -3997,8 +4475,27 @@
       <c r="O33" s="65">
         <v>393</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R33" s="70">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="S33" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="T33" s="77">
+        <v>1</v>
+      </c>
+      <c r="U33" s="65">
+        <v>393</v>
+      </c>
+      <c r="V33" s="54">
+        <v>1</v>
+      </c>
+      <c r="W33" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="54" t="s">
         <v>49</v>
       </c>
@@ -4037,8 +4534,27 @@
         <v>33</v>
       </c>
       <c r="P34" s="60"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R34" s="69">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="S34" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="T34" s="76">
+        <v>1</v>
+      </c>
+      <c r="U34" s="64">
+        <v>33</v>
+      </c>
+      <c r="V34" s="54">
+        <v>1</v>
+      </c>
+      <c r="W34" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="54" t="s">
         <v>169</v>
       </c>
@@ -4076,8 +4592,19 @@
       <c r="P35" s="60" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R35" s="70">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="S35" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="T35" s="77">
+        <v>1</v>
+      </c>
+      <c r="U35" s="65"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="54" t="s">
         <v>20</v>
       </c>
@@ -4119,8 +4646,19 @@
       <c r="P36" s="60" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R36" s="69">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="S36" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="T36" s="76">
+        <v>1</v>
+      </c>
+      <c r="U36" s="64"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="54" t="s">
         <v>121</v>
       </c>
@@ -4153,8 +4691,24 @@
         <v>16</v>
       </c>
       <c r="P37" s="60"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R37" s="70">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="S37" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="T37" s="77">
+        <v>1</v>
+      </c>
+      <c r="U37" s="65">
+        <v>16</v>
+      </c>
+      <c r="V37" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="54" t="s">
         <v>102</v>
       </c>
@@ -4184,8 +4738,19 @@
       <c r="P38" s="63" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R38" s="69">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="S38" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="T38" s="76">
+        <v>1</v>
+      </c>
+      <c r="U38" s="64"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="54" t="s">
         <v>38</v>
       </c>
@@ -4228,8 +4793,19 @@
       <c r="P39" s="63" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R39" s="70">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="S39" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="T39" s="77">
+        <v>1</v>
+      </c>
+      <c r="U39" s="65"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="54" t="s">
         <v>88</v>
       </c>
@@ -4266,8 +4842,24 @@
         <v>41</v>
       </c>
       <c r="P40" s="60"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R40" s="69">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="S40" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="T40" s="76">
+        <v>1</v>
+      </c>
+      <c r="U40" s="64">
+        <v>41</v>
+      </c>
+      <c r="V40" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="54" t="s">
         <v>75</v>
       </c>
@@ -4312,8 +4904,24 @@
         <v>10</v>
       </c>
       <c r="P41" s="60"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R41" s="70">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S41" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="T41" s="77">
+        <v>1</v>
+      </c>
+      <c r="U41" s="65">
+        <v>10</v>
+      </c>
+      <c r="V41" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
         <v>1</v>
       </c>
@@ -4358,8 +4966,24 @@
         <v>18</v>
       </c>
       <c r="P42" s="60"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R42" s="69">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="S42" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="T42" s="76">
+        <v>1</v>
+      </c>
+      <c r="U42" s="64">
+        <v>18</v>
+      </c>
+      <c r="V42" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
         <v>8</v>
       </c>
@@ -4404,8 +5028,27 @@
         <v>10</v>
       </c>
       <c r="P43" s="60"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R43" s="70">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="S43" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="T43" s="77">
+        <v>1</v>
+      </c>
+      <c r="U43" s="65">
+        <v>10</v>
+      </c>
+      <c r="V43" s="54">
+        <v>1</v>
+      </c>
+      <c r="W43" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="54" t="s">
         <v>9</v>
       </c>
@@ -4450,8 +5093,24 @@
         <v>39</v>
       </c>
       <c r="P44" s="60"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R44" s="69">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="S44" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="T44" s="76">
+        <v>1</v>
+      </c>
+      <c r="U44" s="64">
+        <v>39</v>
+      </c>
+      <c r="V44" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
         <v>65</v>
       </c>
@@ -4491,8 +5150,27 @@
         <v>421</v>
       </c>
       <c r="P45" s="60"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R45" s="70">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="S45" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="T45" s="77">
+        <v>1</v>
+      </c>
+      <c r="U45" s="65">
+        <v>421</v>
+      </c>
+      <c r="V45" s="54">
+        <v>1</v>
+      </c>
+      <c r="W45" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="54" t="s">
         <v>82</v>
       </c>
@@ -4537,8 +5215,24 @@
         <v>3</v>
       </c>
       <c r="P46" s="60"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R46" s="69">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="S46" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="T46" s="76">
+        <v>1</v>
+      </c>
+      <c r="U46" s="64">
+        <v>3</v>
+      </c>
+      <c r="V46" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="54" t="s">
         <v>168</v>
       </c>
@@ -4583,8 +5277,24 @@
       <c r="P47" s="60" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R47" s="70">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="S47" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="T47" s="77">
+        <v>1</v>
+      </c>
+      <c r="U47" s="65">
+        <v>88</v>
+      </c>
+      <c r="V47" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B48" s="57" t="s">
         <v>167</v>
       </c>
@@ -4611,8 +5321,19 @@
         <v>150</v>
       </c>
       <c r="P48" s="60"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R48" s="69">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="S48" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="T48" s="76"/>
+      <c r="U48" s="64">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="54" t="s">
         <v>110</v>
       </c>
@@ -4655,8 +5376,19 @@
       <c r="P49" s="60" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R49" s="70">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="S49" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="T49" s="77">
+        <v>1</v>
+      </c>
+      <c r="U49" s="65"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="54" t="s">
         <v>51</v>
       </c>
@@ -4700,8 +5432,24 @@
       <c r="O50" s="64">
         <v>88</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R50" s="69">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="S50" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="T50" s="76">
+        <v>1</v>
+      </c>
+      <c r="U50" s="64">
+        <v>88</v>
+      </c>
+      <c r="V50" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="54" t="s">
         <v>37</v>
       </c>
@@ -4741,8 +5489,19 @@
       <c r="P51" s="60" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R51" s="70">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="S51" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="T51" s="77">
+        <v>1</v>
+      </c>
+      <c r="U51" s="65"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="54" t="s">
         <v>22</v>
       </c>
@@ -4785,8 +5544,24 @@
         <v>20</v>
       </c>
       <c r="P52" s="60"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R52" s="69">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="S52" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="T52" s="76">
+        <v>1</v>
+      </c>
+      <c r="U52" s="64">
+        <v>20</v>
+      </c>
+      <c r="V52" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C53" s="57" t="s">
         <v>166</v>
       </c>
@@ -4814,8 +5589,19 @@
         <v>3</v>
       </c>
       <c r="P53" s="60"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R53" s="70">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="S53" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="T53" s="77"/>
+      <c r="U53" s="65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D54" s="57" t="s">
         <v>165</v>
       </c>
@@ -4839,8 +5625,19 @@
       <c r="O54" s="64">
         <v>33</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R54" s="69">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="S54" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="T54" s="76"/>
+      <c r="U54" s="64">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="54" t="s">
         <v>164</v>
       </c>
@@ -4885,8 +5682,24 @@
         <v>5</v>
       </c>
       <c r="P55" s="60"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R55" s="70">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="S55" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="T55" s="77">
+        <v>1</v>
+      </c>
+      <c r="U55" s="65">
+        <v>5</v>
+      </c>
+      <c r="V55" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="54" t="s">
         <v>15</v>
       </c>
@@ -4929,8 +5742,24 @@
         <v>96</v>
       </c>
       <c r="P56" s="60"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R56" s="69">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="S56" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="T56" s="76">
+        <v>1</v>
+      </c>
+      <c r="U56" s="64">
+        <v>96</v>
+      </c>
+      <c r="V56" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="54" t="s">
         <v>5</v>
       </c>
@@ -4975,8 +5804,24 @@
         <v>44</v>
       </c>
       <c r="P57" s="60"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R57" s="70">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="S57" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="T57" s="77">
+        <v>1</v>
+      </c>
+      <c r="U57" s="65">
+        <v>44</v>
+      </c>
+      <c r="V57" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="54" t="s">
         <v>108</v>
       </c>
@@ -5014,8 +5859,19 @@
       <c r="P58" s="62" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R58" s="69">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="S58" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="T58" s="76">
+        <v>1</v>
+      </c>
+      <c r="U58" s="64"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="54" t="s">
         <v>163</v>
       </c>
@@ -5060,8 +5916,24 @@
         <v>15</v>
       </c>
       <c r="P59" s="60"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R59" s="70">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="S59" s="70" t="s">
+        <v>163</v>
+      </c>
+      <c r="T59" s="77">
+        <v>1</v>
+      </c>
+      <c r="U59" s="65">
+        <v>15</v>
+      </c>
+      <c r="V59" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="54" t="s">
         <v>122</v>
       </c>
@@ -5100,8 +5972,27 @@
         <v>29</v>
       </c>
       <c r="P60" s="60"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R60" s="69">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="S60" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="T60" s="76">
+        <v>1</v>
+      </c>
+      <c r="U60" s="64">
+        <v>29</v>
+      </c>
+      <c r="V60" s="54">
+        <v>1</v>
+      </c>
+      <c r="W60" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="54" t="s">
         <v>39</v>
       </c>
@@ -5145,8 +6036,24 @@
       <c r="O61" s="65">
         <v>70</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R61" s="70">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="S61" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="T61" s="77">
+        <v>1</v>
+      </c>
+      <c r="U61" s="65">
+        <v>70</v>
+      </c>
+      <c r="V61" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="54" t="s">
         <v>162</v>
       </c>
@@ -5188,8 +6095,19 @@
       <c r="P62" s="60" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R62" s="69">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="S62" s="72" t="s">
+        <v>162</v>
+      </c>
+      <c r="T62" s="76">
+        <v>1</v>
+      </c>
+      <c r="U62" s="64"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D63" s="57" t="s">
         <v>161</v>
       </c>
@@ -5219,8 +6137,19 @@
       <c r="P63" s="60" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R63" s="70">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="S63" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="T63" s="77"/>
+      <c r="U63" s="65">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="54" t="s">
         <v>105</v>
       </c>
@@ -5261,8 +6190,24 @@
       <c r="P64" s="60" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R64" s="69">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="S64" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="T64" s="76">
+        <v>1</v>
+      </c>
+      <c r="U64" s="64">
+        <v>33</v>
+      </c>
+      <c r="V64" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D65" s="57" t="s">
         <v>160</v>
       </c>
@@ -5292,8 +6237,22 @@
         <v>10</v>
       </c>
       <c r="P65" s="60"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R65" s="70">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="S65" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="T65" s="77"/>
+      <c r="U65" s="65">
+        <v>10</v>
+      </c>
+      <c r="X65" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="54" t="s">
         <v>25</v>
       </c>
@@ -5332,8 +6291,24 @@
         <v>46</v>
       </c>
       <c r="P66" s="60"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R66" s="69">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="S66" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="T66" s="76">
+        <v>1</v>
+      </c>
+      <c r="U66" s="64">
+        <v>46</v>
+      </c>
+      <c r="V66" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="54" t="s">
         <v>10</v>
       </c>
@@ -5378,8 +6353,24 @@
         <v>280</v>
       </c>
       <c r="P67" s="60"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R67" s="70">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="S67" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="T67" s="77">
+        <v>1</v>
+      </c>
+      <c r="U67" s="65">
+        <v>280</v>
+      </c>
+      <c r="V67" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="54" t="s">
         <v>159</v>
       </c>
@@ -5396,7 +6387,7 @@
         <v>0</v>
       </c>
       <c r="H68" s="69">
-        <f t="shared" ref="H68:H124" si="1">H67+1</f>
+        <f t="shared" ref="H68:H124" si="2">H67+1</f>
         <v>67</v>
       </c>
       <c r="I68" s="72" t="s">
@@ -5416,8 +6407,24 @@
         <v>13</v>
       </c>
       <c r="P68" s="60"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R68" s="69">
+        <f t="shared" ref="R68:R124" si="3">R67+1</f>
+        <v>67</v>
+      </c>
+      <c r="S68" s="72" t="s">
+        <v>159</v>
+      </c>
+      <c r="T68" s="76">
+        <v>1</v>
+      </c>
+      <c r="U68" s="64">
+        <v>13</v>
+      </c>
+      <c r="V68" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D69" s="57" t="s">
         <v>158</v>
       </c>
@@ -5428,7 +6435,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
       <c r="I69" s="70" t="s">
@@ -5446,8 +6453,19 @@
       <c r="O69" s="65">
         <v>11</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R69" s="70">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="S69" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="T69" s="77"/>
+      <c r="U69" s="65">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="54" t="s">
         <v>6</v>
       </c>
@@ -5467,7 +6485,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="I70" s="72" t="s">
@@ -5492,8 +6510,24 @@
         <v>474</v>
       </c>
       <c r="P70" s="60"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R70" s="69">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="S70" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="T70" s="76">
+        <v>1</v>
+      </c>
+      <c r="U70" s="64">
+        <v>474</v>
+      </c>
+      <c r="V70" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="54" t="s">
         <v>7</v>
       </c>
@@ -5513,7 +6547,7 @@
         <v>1</v>
       </c>
       <c r="H71" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="I71" s="70" t="s">
@@ -5538,8 +6572,24 @@
         <v>3</v>
       </c>
       <c r="P71" s="60"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R71" s="70">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="S71" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="T71" s="77">
+        <v>1</v>
+      </c>
+      <c r="U71" s="65">
+        <v>3</v>
+      </c>
+      <c r="V71" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D72" s="57" t="s">
         <v>157</v>
       </c>
@@ -5550,7 +6600,7 @@
         <v>0</v>
       </c>
       <c r="H72" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="I72" s="72" t="s">
@@ -5564,8 +6614,19 @@
         <v>2</v>
       </c>
       <c r="P72" s="60"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R72" s="69">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="S72" s="72" t="s">
+        <v>157</v>
+      </c>
+      <c r="T72" s="76"/>
+      <c r="U72" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="54" t="s">
         <v>33</v>
       </c>
@@ -5585,7 +6646,7 @@
         <v>0</v>
       </c>
       <c r="H73" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="I73" s="70" t="s">
@@ -5607,8 +6668,24 @@
       <c r="O73" s="65">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R73" s="70">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="S73" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="T73" s="77">
+        <v>1</v>
+      </c>
+      <c r="U73" s="65">
+        <v>13</v>
+      </c>
+      <c r="V73" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B74" s="57" t="s">
         <v>156</v>
       </c>
@@ -5619,7 +6696,7 @@
         <v>1</v>
       </c>
       <c r="H74" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="I74" s="72" t="s">
@@ -5635,8 +6712,19 @@
         <v>73</v>
       </c>
       <c r="P74" s="60"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R74" s="69">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="S74" s="72" t="s">
+        <v>156</v>
+      </c>
+      <c r="T74" s="76"/>
+      <c r="U74" s="64">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="54" t="s">
         <v>155</v>
       </c>
@@ -5650,7 +6738,7 @@
         <v>1</v>
       </c>
       <c r="H75" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="I75" s="70" t="s">
@@ -5671,8 +6759,27 @@
         <v>3</v>
       </c>
       <c r="P75" s="60"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R75" s="70">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="S75" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="T75" s="77">
+        <v>1</v>
+      </c>
+      <c r="U75" s="65">
+        <v>3</v>
+      </c>
+      <c r="V75" s="54">
+        <v>1</v>
+      </c>
+      <c r="W75" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="54" t="s">
         <v>154</v>
       </c>
@@ -5689,7 +6796,7 @@
         <v>1</v>
       </c>
       <c r="H76" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="I76" s="72" t="s">
@@ -5711,8 +6818,24 @@
         <v>13</v>
       </c>
       <c r="P76" s="60"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R76" s="69">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="S76" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="T76" s="76">
+        <v>1</v>
+      </c>
+      <c r="U76" s="64">
+        <v>13</v>
+      </c>
+      <c r="V76" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="54" t="s">
         <v>48</v>
       </c>
@@ -5732,7 +6855,7 @@
         <v>1</v>
       </c>
       <c r="H77" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
       <c r="I77" s="70" t="s">
@@ -5757,8 +6880,24 @@
         <v>7</v>
       </c>
       <c r="P77" s="60"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R77" s="70">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="S77" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="T77" s="77">
+        <v>1</v>
+      </c>
+      <c r="U77" s="65">
+        <v>7</v>
+      </c>
+      <c r="V77" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="54" t="s">
         <v>153</v>
       </c>
@@ -5769,7 +6908,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="I78" s="72" t="s">
@@ -5785,8 +6924,24 @@
         <v>85</v>
       </c>
       <c r="P78" s="60"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R78" s="69">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="S78" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="T78" s="76">
+        <v>1</v>
+      </c>
+      <c r="U78" s="64">
+        <v>85</v>
+      </c>
+      <c r="V78" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D79" s="57" t="s">
         <v>152</v>
       </c>
@@ -5797,7 +6952,7 @@
         <v>0</v>
       </c>
       <c r="H79" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
       <c r="I79" s="70" t="s">
@@ -5814,8 +6969,22 @@
         <v>11</v>
       </c>
       <c r="P79" s="60"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R79" s="70">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="S79" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="T79" s="77"/>
+      <c r="U79" s="65">
+        <v>11</v>
+      </c>
+      <c r="W79" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D80" s="57" t="s">
         <v>151</v>
       </c>
@@ -5826,7 +6995,7 @@
         <v>0</v>
       </c>
       <c r="H80" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="I80" s="72" t="s">
@@ -5842,8 +7011,19 @@
       <c r="P80" s="60" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R80" s="69">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="S80" s="72" t="s">
+        <v>151</v>
+      </c>
+      <c r="T80" s="76"/>
+      <c r="U80" s="64">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="54" t="s">
         <v>81</v>
       </c>
@@ -5860,7 +7040,7 @@
         <v>1</v>
       </c>
       <c r="H81" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="I81" s="70" t="s">
@@ -5883,8 +7063,24 @@
         <v>36</v>
       </c>
       <c r="P81" s="60"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R81" s="70">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="S81" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="T81" s="77">
+        <v>1</v>
+      </c>
+      <c r="U81" s="65">
+        <v>36</v>
+      </c>
+      <c r="V81" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D82" s="57" t="s">
         <v>150</v>
       </c>
@@ -5895,7 +7091,7 @@
         <v>0</v>
       </c>
       <c r="H82" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
       <c r="I82" s="72" t="s">
@@ -5911,8 +7107,19 @@
       <c r="P82" s="60" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R82" s="69">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="S82" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="T82" s="76"/>
+      <c r="U82" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="54" t="s">
         <v>29</v>
       </c>
@@ -5932,7 +7139,7 @@
         <v>1</v>
       </c>
       <c r="H83" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="I83" s="70" t="s">
@@ -5957,8 +7164,24 @@
         <v>21</v>
       </c>
       <c r="P83" s="60"/>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R83" s="70">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="S83" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="T83" s="77">
+        <v>1</v>
+      </c>
+      <c r="U83" s="65">
+        <v>21</v>
+      </c>
+      <c r="V83" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="54" t="s">
         <v>93</v>
       </c>
@@ -5975,7 +7198,7 @@
         <v>0</v>
       </c>
       <c r="H84" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
       <c r="I84" s="72" t="s">
@@ -5995,8 +7218,27 @@
         <v>393</v>
       </c>
       <c r="P84" s="60"/>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R84" s="69">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="S84" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="T84" s="76">
+        <v>1</v>
+      </c>
+      <c r="U84" s="64">
+        <v>393</v>
+      </c>
+      <c r="V84" s="54">
+        <v>1</v>
+      </c>
+      <c r="W84" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="54" t="s">
         <v>16</v>
       </c>
@@ -6016,7 +7258,7 @@
         <v>0</v>
       </c>
       <c r="H85" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
       <c r="I85" s="70" t="s">
@@ -6039,8 +7281,24 @@
         <v>2</v>
       </c>
       <c r="P85" s="60"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R85" s="70">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="S85" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="T85" s="77">
+        <v>1</v>
+      </c>
+      <c r="U85" s="65">
+        <v>2</v>
+      </c>
+      <c r="V85" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="54" t="s">
         <v>17</v>
       </c>
@@ -6060,7 +7318,7 @@
         <v>0</v>
       </c>
       <c r="H86" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="I86" s="72" t="s">
@@ -6083,8 +7341,24 @@
         <v>73</v>
       </c>
       <c r="P86" s="60"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R86" s="69">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="S86" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="T86" s="76">
+        <v>1</v>
+      </c>
+      <c r="U86" s="64">
+        <v>73</v>
+      </c>
+      <c r="V86" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" s="54" t="s">
         <v>47</v>
       </c>
@@ -6104,7 +7378,7 @@
         <v>1</v>
       </c>
       <c r="H87" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="I87" s="70" t="s">
@@ -6129,8 +7403,24 @@
         <v>11</v>
       </c>
       <c r="P87" s="60"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R87" s="70">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="S87" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="T87" s="77">
+        <v>1</v>
+      </c>
+      <c r="U87" s="65">
+        <v>11</v>
+      </c>
+      <c r="V87" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="54" t="s">
         <v>120</v>
       </c>
@@ -6144,7 +7434,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="I88" s="72" t="s">
@@ -6162,8 +7452,27 @@
       <c r="O88" s="64">
         <v>251</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R88" s="69">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="S88" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="T88" s="76">
+        <v>1</v>
+      </c>
+      <c r="U88" s="64">
+        <v>251</v>
+      </c>
+      <c r="V88" s="54">
+        <v>1</v>
+      </c>
+      <c r="W88" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D89" s="57" t="s">
         <v>149</v>
       </c>
@@ -6174,7 +7483,7 @@
         <v>0</v>
       </c>
       <c r="H89" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="I89" s="70" t="s">
@@ -6193,8 +7502,19 @@
       <c r="P89" s="60" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R89" s="70">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+      <c r="S89" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="T89" s="77"/>
+      <c r="U89" s="65">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" s="54" t="s">
         <v>103</v>
       </c>
@@ -6211,7 +7531,7 @@
         <v>1</v>
       </c>
       <c r="H90" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
       <c r="I90" s="72" t="s">
@@ -6233,8 +7553,27 @@
         <v>619</v>
       </c>
       <c r="P90" s="60"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R90" s="69">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="S90" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="T90" s="76">
+        <v>1</v>
+      </c>
+      <c r="U90" s="64">
+        <v>619</v>
+      </c>
+      <c r="V90" s="54">
+        <v>1</v>
+      </c>
+      <c r="W90" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" s="54" t="s">
         <v>104</v>
       </c>
@@ -6251,7 +7590,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="I91" s="70" t="s">
@@ -6274,8 +7613,24 @@
         <v>230</v>
       </c>
       <c r="P91" s="60"/>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R91" s="70">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="S91" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="T91" s="77">
+        <v>1</v>
+      </c>
+      <c r="U91" s="65">
+        <v>230</v>
+      </c>
+      <c r="V91" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" s="54" t="s">
         <v>148</v>
       </c>
@@ -6292,7 +7647,7 @@
         <v>1</v>
       </c>
       <c r="H92" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91</v>
       </c>
       <c r="I92" s="72" t="s">
@@ -6314,8 +7669,24 @@
         <v>2</v>
       </c>
       <c r="P92" s="60"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R92" s="69">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="S92" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="T92" s="76">
+        <v>1</v>
+      </c>
+      <c r="U92" s="64">
+        <v>2</v>
+      </c>
+      <c r="V92" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" s="54" t="s">
         <v>79</v>
       </c>
@@ -6335,7 +7706,7 @@
         <v>1</v>
       </c>
       <c r="H93" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
       <c r="I93" s="70" t="s">
@@ -6360,8 +7731,27 @@
         <v>37</v>
       </c>
       <c r="P93" s="60"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R93" s="70">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+      <c r="S93" s="70" t="s">
+        <v>79</v>
+      </c>
+      <c r="T93" s="77">
+        <v>1</v>
+      </c>
+      <c r="U93" s="65">
+        <v>37</v>
+      </c>
+      <c r="V93" s="54">
+        <v>1</v>
+      </c>
+      <c r="W93" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" s="54" t="s">
         <v>94</v>
       </c>
@@ -6378,7 +7768,7 @@
         <v>1</v>
       </c>
       <c r="H94" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="I94" s="72" t="s">
@@ -6400,8 +7790,27 @@
         <v>46</v>
       </c>
       <c r="P94" s="60"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R94" s="69">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="S94" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="T94" s="76">
+        <v>1</v>
+      </c>
+      <c r="U94" s="64">
+        <v>46</v>
+      </c>
+      <c r="V94" s="54">
+        <v>1</v>
+      </c>
+      <c r="W94" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" s="54" t="s">
         <v>40</v>
       </c>
@@ -6421,7 +7830,7 @@
         <v>1</v>
       </c>
       <c r="H95" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94</v>
       </c>
       <c r="I95" s="70" t="s">
@@ -6445,8 +7854,27 @@
       <c r="O95" s="65">
         <v>313</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R95" s="70">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+      <c r="S95" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="T95" s="77">
+        <v>1</v>
+      </c>
+      <c r="U95" s="65">
+        <v>313</v>
+      </c>
+      <c r="V95" s="54">
+        <v>1</v>
+      </c>
+      <c r="W95" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" s="54" t="s">
         <v>147</v>
       </c>
@@ -6460,7 +7888,7 @@
         <v>1</v>
       </c>
       <c r="H96" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="I96" s="72" t="s">
@@ -6478,8 +7906,24 @@
       <c r="O96" s="64">
         <v>10</v>
       </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R96" s="69">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="S96" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="T96" s="76">
+        <v>1</v>
+      </c>
+      <c r="U96" s="64">
+        <v>10</v>
+      </c>
+      <c r="V96" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D97" s="57" t="s">
         <v>146</v>
       </c>
@@ -6490,7 +7934,7 @@
         <v>1</v>
       </c>
       <c r="H97" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="I97" s="70" t="s">
@@ -6508,8 +7952,19 @@
       <c r="O97" s="65">
         <v>23</v>
       </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R97" s="70">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="S97" s="70" t="s">
+        <v>146</v>
+      </c>
+      <c r="T97" s="77"/>
+      <c r="U97" s="65">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" s="54" t="s">
         <v>24</v>
       </c>
@@ -6529,7 +7984,7 @@
         <v>1</v>
       </c>
       <c r="H98" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="I98" s="72" t="s">
@@ -6553,8 +8008,24 @@
       <c r="O98" s="64">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R98" s="69">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="S98" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="T98" s="76">
+        <v>1</v>
+      </c>
+      <c r="U98" s="64">
+        <v>2</v>
+      </c>
+      <c r="V98" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" s="54" t="s">
         <v>34</v>
       </c>
@@ -6574,7 +8045,7 @@
         <v>1</v>
       </c>
       <c r="H99" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="I99" s="70" t="s">
@@ -6598,8 +8069,24 @@
       <c r="O99" s="65">
         <v>16</v>
       </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R99" s="70">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="S99" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="T99" s="77">
+        <v>1</v>
+      </c>
+      <c r="U99" s="65">
+        <v>16</v>
+      </c>
+      <c r="V99" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="54" t="s">
         <v>50</v>
       </c>
@@ -6616,7 +8103,7 @@
         <v>0</v>
       </c>
       <c r="H100" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="I100" s="72" t="s">
@@ -6635,8 +8122,24 @@
       <c r="O100" s="64">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R100" s="69">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+      <c r="S100" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="T100" s="76">
+        <v>1</v>
+      </c>
+      <c r="U100" s="64">
+        <v>5</v>
+      </c>
+      <c r="V100" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" s="54" t="s">
         <v>26</v>
       </c>
@@ -6656,7 +8159,7 @@
         <v>1</v>
       </c>
       <c r="H101" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="I101" s="70" t="s">
@@ -6680,8 +8183,24 @@
       <c r="O101" s="65">
         <v>93</v>
       </c>
-    </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R101" s="70">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="S101" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="T101" s="77">
+        <v>1</v>
+      </c>
+      <c r="U101" s="65">
+        <v>93</v>
+      </c>
+      <c r="V101" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" s="54" t="s">
         <v>123</v>
       </c>
@@ -6698,7 +8217,7 @@
         <v>0</v>
       </c>
       <c r="H102" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="I102" s="72" t="s">
@@ -6717,8 +8236,24 @@
       <c r="O102" s="64">
         <v>21</v>
       </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R102" s="69">
+        <f t="shared" si="3"/>
+        <v>101</v>
+      </c>
+      <c r="S102" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="T102" s="76">
+        <v>1</v>
+      </c>
+      <c r="U102" s="64">
+        <v>21</v>
+      </c>
+      <c r="V102" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" s="54" t="s">
         <v>19</v>
       </c>
@@ -6738,7 +8273,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="I103" s="70" t="s">
@@ -6762,8 +8297,24 @@
       <c r="O103" s="65">
         <v>11</v>
       </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R103" s="70">
+        <f t="shared" si="3"/>
+        <v>102</v>
+      </c>
+      <c r="S103" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="T103" s="77">
+        <v>1</v>
+      </c>
+      <c r="U103" s="65">
+        <v>11</v>
+      </c>
+      <c r="V103" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" s="54" t="s">
         <v>115</v>
       </c>
@@ -6780,7 +8331,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="I104" s="72" t="s">
@@ -6801,8 +8352,24 @@
       <c r="O104" s="64">
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R104" s="69">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
+      <c r="S104" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="T104" s="76">
+        <v>1</v>
+      </c>
+      <c r="U104" s="64">
+        <v>7</v>
+      </c>
+      <c r="V104" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" s="54" t="s">
         <v>80</v>
       </c>
@@ -6816,7 +8383,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="I105" s="70" t="s">
@@ -6836,8 +8403,27 @@
       <c r="O105" s="65">
         <v>572</v>
       </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R105" s="70">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+      <c r="S105" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="T105" s="77">
+        <v>1</v>
+      </c>
+      <c r="U105" s="65">
+        <v>572</v>
+      </c>
+      <c r="V105" s="54">
+        <v>1</v>
+      </c>
+      <c r="W105" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" s="54" t="s">
         <v>85</v>
       </c>
@@ -6857,7 +8443,7 @@
         <v>0</v>
       </c>
       <c r="H106" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="I106" s="72" t="s">
@@ -6879,8 +8465,24 @@
       <c r="O106" s="64">
         <v>29</v>
       </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R106" s="69">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="S106" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="T106" s="76">
+        <v>1</v>
+      </c>
+      <c r="U106" s="64">
+        <v>29</v>
+      </c>
+      <c r="V106" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D107" s="57" t="s">
         <v>86</v>
       </c>
@@ -6891,7 +8493,7 @@
         <v>0</v>
       </c>
       <c r="H107" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="I107" s="70" t="s">
@@ -6907,8 +8509,19 @@
       <c r="O107" s="65">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R107" s="70">
+        <f t="shared" si="3"/>
+        <v>106</v>
+      </c>
+      <c r="S107" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="T107" s="77"/>
+      <c r="U107" s="65">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" s="54" t="s">
         <v>11</v>
       </c>
@@ -6928,7 +8541,7 @@
         <v>1</v>
       </c>
       <c r="H108" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="I108" s="72" t="s">
@@ -6952,8 +8565,27 @@
       <c r="O108" s="64">
         <v>153</v>
       </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R108" s="69">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+      <c r="S108" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="T108" s="76">
+        <v>1</v>
+      </c>
+      <c r="U108" s="64">
+        <v>153</v>
+      </c>
+      <c r="V108" s="54">
+        <v>1</v>
+      </c>
+      <c r="W108" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" s="54" t="s">
         <v>145</v>
       </c>
@@ -6964,7 +8596,7 @@
         <v>0</v>
       </c>
       <c r="H109" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="I109" s="70" t="s">
@@ -6981,8 +8613,19 @@
       <c r="P109" s="62" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R109" s="70">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="S109" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="T109" s="77">
+        <v>1</v>
+      </c>
+      <c r="U109" s="65"/>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D110" s="57" t="s">
         <v>144</v>
       </c>
@@ -6993,7 +8636,7 @@
         <v>1</v>
       </c>
       <c r="H110" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109</v>
       </c>
       <c r="I110" s="72" t="s">
@@ -7008,8 +8651,19 @@
       <c r="O110" s="64">
         <v>10</v>
       </c>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R110" s="69">
+        <f t="shared" si="3"/>
+        <v>109</v>
+      </c>
+      <c r="S110" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="T110" s="76"/>
+      <c r="U110" s="64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" s="54" t="s">
         <v>28</v>
       </c>
@@ -7029,7 +8683,7 @@
         <v>1</v>
       </c>
       <c r="H111" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="I111" s="70" t="s">
@@ -7053,8 +8707,27 @@
       <c r="O111" s="65">
         <v>205</v>
       </c>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R111" s="70">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="S111" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="T111" s="77">
+        <v>1</v>
+      </c>
+      <c r="U111" s="65">
+        <v>205</v>
+      </c>
+      <c r="V111" s="54">
+        <v>1</v>
+      </c>
+      <c r="W111" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" s="54" t="s">
         <v>53</v>
       </c>
@@ -7074,7 +8747,7 @@
         <v>1</v>
       </c>
       <c r="H112" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="I112" s="72" t="s">
@@ -7098,8 +8771,24 @@
       <c r="O112" s="64">
         <v>13</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R112" s="69">
+        <f t="shared" si="3"/>
+        <v>111</v>
+      </c>
+      <c r="S112" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="T112" s="76">
+        <v>1</v>
+      </c>
+      <c r="U112" s="64">
+        <v>13</v>
+      </c>
+      <c r="V112" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D113" s="57" t="s">
         <v>35</v>
       </c>
@@ -7110,7 +8799,7 @@
         <v>1</v>
       </c>
       <c r="H113" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112</v>
       </c>
       <c r="I113" s="70" t="s">
@@ -7128,8 +8817,19 @@
       <c r="O113" s="65">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R113" s="70">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
+      <c r="S113" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="T113" s="77"/>
+      <c r="U113" s="65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="54" t="s">
         <v>30</v>
       </c>
@@ -7149,7 +8849,7 @@
         <v>1</v>
       </c>
       <c r="H114" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
       <c r="I114" s="72" t="s">
@@ -7173,8 +8873,24 @@
       <c r="O114" s="64">
         <v>109</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R114" s="69">
+        <f t="shared" si="3"/>
+        <v>113</v>
+      </c>
+      <c r="S114" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="T114" s="76">
+        <v>1</v>
+      </c>
+      <c r="U114" s="64">
+        <v>109</v>
+      </c>
+      <c r="V114" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B115" s="57" t="s">
         <v>143</v>
       </c>
@@ -7185,7 +8901,7 @@
         <v>1</v>
       </c>
       <c r="H115" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>114</v>
       </c>
       <c r="I115" s="70" t="s">
@@ -7203,8 +8919,19 @@
       <c r="O115" s="65">
         <v>184</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R115" s="70">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="S115" s="70" t="s">
+        <v>143</v>
+      </c>
+      <c r="T115" s="77"/>
+      <c r="U115" s="65">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" s="54" t="s">
         <v>45</v>
       </c>
@@ -7221,7 +8948,7 @@
         <v>0</v>
       </c>
       <c r="H116" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="I116" s="72" t="s">
@@ -7240,8 +8967,24 @@
       <c r="O116" s="64">
         <v>494</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R116" s="69">
+        <f t="shared" si="3"/>
+        <v>115</v>
+      </c>
+      <c r="S116" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="T116" s="76">
+        <v>1</v>
+      </c>
+      <c r="U116" s="64">
+        <v>494</v>
+      </c>
+      <c r="V116" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="54" t="s">
         <v>55</v>
       </c>
@@ -7255,7 +8998,7 @@
         <v>1</v>
       </c>
       <c r="H117" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="I117" s="70" t="s">
@@ -7275,8 +9018,24 @@
       <c r="O117" s="65">
         <v>300</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R117" s="70">
+        <f t="shared" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="S117" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="T117" s="77">
+        <v>1</v>
+      </c>
+      <c r="U117" s="65">
+        <v>300</v>
+      </c>
+      <c r="V117" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B118" s="57" t="s">
         <v>142</v>
       </c>
@@ -7287,7 +9046,7 @@
         <v>1</v>
       </c>
       <c r="H118" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
       <c r="I118" s="72" t="s">
@@ -7302,8 +9061,19 @@
       <c r="O118" s="64">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R118" s="69">
+        <f t="shared" si="3"/>
+        <v>117</v>
+      </c>
+      <c r="S118" s="72" t="s">
+        <v>142</v>
+      </c>
+      <c r="T118" s="76"/>
+      <c r="U118" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="54" t="s">
         <v>111</v>
       </c>
@@ -7320,7 +9090,7 @@
         <v>1</v>
       </c>
       <c r="H119" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="I119" s="70" t="s">
@@ -7342,8 +9112,27 @@
       <c r="O119" s="65">
         <v>24</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R119" s="70">
+        <f t="shared" si="3"/>
+        <v>118</v>
+      </c>
+      <c r="S119" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="T119" s="77">
+        <v>1</v>
+      </c>
+      <c r="U119" s="65">
+        <v>24</v>
+      </c>
+      <c r="V119" s="54">
+        <v>1</v>
+      </c>
+      <c r="W119" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="54" t="s">
         <v>42</v>
       </c>
@@ -7363,7 +9152,7 @@
         <v>1</v>
       </c>
       <c r="H120" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119</v>
       </c>
       <c r="I120" s="72" t="s">
@@ -7387,8 +9176,27 @@
       <c r="O120" s="64">
         <v>73</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R120" s="69">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+      <c r="S120" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="T120" s="76">
+        <v>1</v>
+      </c>
+      <c r="U120" s="64">
+        <v>73</v>
+      </c>
+      <c r="V120" s="54">
+        <v>1</v>
+      </c>
+      <c r="W120" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="54" t="s">
         <v>12</v>
       </c>
@@ -7408,7 +9216,7 @@
         <v>0</v>
       </c>
       <c r="H121" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="I121" s="70" t="s">
@@ -7430,8 +9238,24 @@
       <c r="O121" s="65">
         <v>5</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R121" s="70">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="S121" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="T121" s="77">
+        <v>1</v>
+      </c>
+      <c r="U121" s="65">
+        <v>5</v>
+      </c>
+      <c r="V121" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B122" s="57" t="s">
         <v>141</v>
       </c>
@@ -7442,7 +9266,7 @@
         <v>1</v>
       </c>
       <c r="H122" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="I122" s="72" t="s">
@@ -7457,8 +9281,22 @@
       <c r="O122" s="64">
         <v>13</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R122" s="69">
+        <f t="shared" si="3"/>
+        <v>121</v>
+      </c>
+      <c r="S122" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="T122" s="76"/>
+      <c r="U122" s="64">
+        <v>13</v>
+      </c>
+      <c r="X122" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="54" t="s">
         <v>126</v>
       </c>
@@ -7472,7 +9310,7 @@
         <v>1</v>
       </c>
       <c r="H123" s="70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122</v>
       </c>
       <c r="I123" s="70" t="s">
@@ -7492,8 +9330,24 @@
       <c r="O123" s="65">
         <v>15</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R123" s="70">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="S123" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="T123" s="77">
+        <v>1</v>
+      </c>
+      <c r="U123" s="65">
+        <v>15</v>
+      </c>
+      <c r="V123" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D124" s="57" t="s">
         <v>140</v>
       </c>
@@ -7504,7 +9358,7 @@
         <v>1</v>
       </c>
       <c r="H124" s="69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123</v>
       </c>
       <c r="I124" s="72" t="s">
@@ -7519,8 +9373,19 @@
       <c r="O124" s="64">
         <v>668</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R124" s="69">
+        <f t="shared" si="3"/>
+        <v>123</v>
+      </c>
+      <c r="S124" s="72" t="s">
+        <v>140</v>
+      </c>
+      <c r="T124" s="76"/>
+      <c r="U124" s="64">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="53">
         <f>COUNTA(A2:A123)</f>
         <v>94</v>
@@ -7578,8 +9443,29 @@
         <f>COUNTA(O2:O124)</f>
         <v>110</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R125" s="71"/>
+      <c r="S125" s="74">
+        <f>COUNTA(S2:S124)</f>
+        <v>123</v>
+      </c>
+      <c r="T125" s="78">
+        <f>SUM(T2:T124)</f>
+        <v>94</v>
+      </c>
+      <c r="U125" s="67">
+        <f>COUNTA(U2:U124)</f>
+        <v>110</v>
+      </c>
+      <c r="V125" s="54">
+        <f>SUM(V2:V124)</f>
+        <v>83</v>
+      </c>
+      <c r="W125" s="54">
+        <f>SUM(W2:W124)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="53" t="s">
         <v>139</v>
       </c>

</xml_diff>